<commit_message>
Additional info added to file
</commit_message>
<xml_diff>
--- a/ExpOverview.xlsx
+++ b/ExpOverview.xlsx
@@ -1,34 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mvanswieten\Documents\GitHub_repositories\3d-point-clouds\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A2C0BD-207A-44E9-8F92-B446569164EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{8E2A9C72-EEC9-47AC-8B0E-8FA68B04BC70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23028" windowHeight="12228" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="732" windowWidth="23028" windowHeight="12228" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="WT" sheetId="3" r:id="rId1"/>
-    <sheet name="transgenic" sheetId="1" r:id="rId2"/>
-    <sheet name="Nex-cKO" sheetId="2" r:id="rId3"/>
-    <sheet name="Rat_SM" sheetId="4" r:id="rId4"/>
-    <sheet name="Rat_barrel" sheetId="5" r:id="rId5"/>
-    <sheet name="Rat_cortex" sheetId="6" r:id="rId6"/>
-    <sheet name="Rat_SS" sheetId="7" r:id="rId7"/>
+    <sheet name="README" sheetId="8" r:id="rId1"/>
+    <sheet name="WT" sheetId="3" r:id="rId2"/>
+    <sheet name="transgenic" sheetId="1" r:id="rId3"/>
+    <sheet name="Nex-cKO" sheetId="2" r:id="rId4"/>
+    <sheet name="Rat_SM" sheetId="4" r:id="rId5"/>
+    <sheet name="Rat_barrel" sheetId="5" r:id="rId6"/>
+    <sheet name="Rat_cortex" sheetId="6" r:id="rId7"/>
+    <sheet name="Rat_SS" sheetId="7" r:id="rId8"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'Nex-cKO'!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Rat_barrel!$B$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Rat_cortex!$A$1:$L$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Rat_SM!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Rat_SS!$A$1:$K$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">transgenic!$A$1:$M$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">WT!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'Nex-cKO'!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="5" hidden="1">Rat_barrel!$B$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Rat_cortex!$A$1:$L$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Rat_SM!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">Rat_SS!$A$1:$K$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">transgenic!$A$1:$M$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">WT!$A$1:$L$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -51,7 +52,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="337">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1897" uniqueCount="352">
   <si>
     <t>expNumber</t>
   </si>
@@ -1062,6 +1063,51 @@
   </si>
   <si>
     <t>R124_BDA</t>
+  </si>
+  <si>
+    <t>This overview Table contains the following metadata for each dataset:</t>
+  </si>
+  <si>
+    <t>Experiment number</t>
+  </si>
+  <si>
+    <t>Experiment name</t>
+  </si>
+  <si>
+    <t>genotype/strain</t>
+  </si>
+  <si>
+    <t>Genotype and strain name</t>
+  </si>
+  <si>
+    <t>Sex of the animal</t>
+  </si>
+  <si>
+    <t>Age at tracer injection timepoint</t>
+  </si>
+  <si>
+    <t>Age at euthanasia</t>
+  </si>
+  <si>
+    <t>Abreviated name of the brain region where the tracer was injected</t>
+  </si>
+  <si>
+    <t>Full name of the brain region where the tracer was injected</t>
+  </si>
+  <si>
+    <t>Hemisphere of tracer injection</t>
+  </si>
+  <si>
+    <t>Color name of the injection site and point clouds representing anterogradely labelled axons</t>
+  </si>
+  <si>
+    <t>RGB color code</t>
+  </si>
+  <si>
+    <t>Color coding of the injection site according to their distance from the anterolateral cerebral cortex towards frontal, medial, and occipital locations (fig3 A, C)</t>
+  </si>
+  <si>
+    <t>1:  (RGB 250 250 110); 2: ( RGB 156 223 124); 3: ( RGB 74 189 140); 4: ( RGB 0 150 142); 5: ( RGB 16 110 124); 6: (RGB 42 72 88)</t>
   </si>
 </sst>
 </file>
@@ -1149,7 +1195,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1198,13 +1244,99 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1268,6 +1400,53 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -1287,10 +1466,65 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>6169167</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>47245</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDDAF37C-3EBB-4C06-87B0-23A750B5836A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1676400" y="3213100"/>
+          <a:ext cx="7388367" cy="599695"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1328,7 +1562,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1434,7 +1668,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1576,33 +1810,415 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3006A074-504F-4808-A627-E30A370247A1}">
+  <dimension ref="A2:K25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D32" sqref="D32:D33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <cols>
+    <col min="1" max="1" width="24" customWidth="1"/>
+    <col min="4" max="4" width="119.7890625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A2" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="B2" s="27"/>
+      <c r="C2" s="27"/>
+      <c r="D2" s="27"/>
+      <c r="E2" s="28"/>
+      <c r="F2" s="28"/>
+      <c r="G2" s="28"/>
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="29"/>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A3" s="28"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
+      <c r="E3" s="28"/>
+      <c r="F3" s="28"/>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="29"/>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A4" s="26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4" s="30" t="s">
+        <v>338</v>
+      </c>
+      <c r="C4" s="31"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="28"/>
+      <c r="F4" s="28"/>
+      <c r="G4" s="28"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="29"/>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A5" s="26" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="30" t="s">
+        <v>339</v>
+      </c>
+      <c r="C5" s="31"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="28"/>
+      <c r="F5" s="28"/>
+      <c r="G5" s="28"/>
+      <c r="H5" s="28"/>
+      <c r="I5" s="28"/>
+      <c r="J5" s="28"/>
+      <c r="K5" s="29"/>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A6" s="26" t="s">
+        <v>340</v>
+      </c>
+      <c r="B6" s="30" t="s">
+        <v>341</v>
+      </c>
+      <c r="C6" s="31"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="28"/>
+      <c r="F6" s="28"/>
+      <c r="G6" s="28"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="28"/>
+      <c r="J6" s="28"/>
+      <c r="K6" s="29"/>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A7" s="26" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" s="30" t="s">
+        <v>342</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
+      <c r="I7" s="28"/>
+      <c r="J7" s="28"/>
+      <c r="K7" s="29"/>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A8" s="26" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="30" t="s">
+        <v>343</v>
+      </c>
+      <c r="C8" s="31"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="29"/>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A9" s="26" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="30" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" s="31"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="28"/>
+      <c r="F9" s="28"/>
+      <c r="G9" s="28"/>
+      <c r="H9" s="28"/>
+      <c r="I9" s="28"/>
+      <c r="J9" s="28"/>
+      <c r="K9" s="29"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A10" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="C10" s="31"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A11" s="26" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="33" t="s">
+        <v>346</v>
+      </c>
+      <c r="C11" s="34"/>
+      <c r="D11" s="35"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A12" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="30" t="s">
+        <v>347</v>
+      </c>
+      <c r="C12" s="31"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A13" s="17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="30" t="s">
+        <v>348</v>
+      </c>
+      <c r="C13" s="31"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A14" s="36" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" s="37" t="s">
+        <v>349</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="39"/>
+      <c r="E14" s="28"/>
+      <c r="F14" s="28"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
+    </row>
+    <row r="15" spans="1:11" ht="21" customHeight="1" x14ac:dyDescent="0.55000000000000004">
+      <c r="A15" s="44" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="37" t="s">
+        <v>350</v>
+      </c>
+      <c r="C15" s="38"/>
+      <c r="D15" s="39"/>
+      <c r="E15" s="28"/>
+      <c r="F15" s="28"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A16" s="45"/>
+      <c r="B16" s="40" t="s">
+        <v>351</v>
+      </c>
+      <c r="C16" s="41"/>
+      <c r="D16" s="42"/>
+      <c r="E16" s="28"/>
+      <c r="F16" s="28"/>
+      <c r="G16" s="28"/>
+      <c r="H16" s="28"/>
+      <c r="I16" s="28"/>
+      <c r="J16" s="28"/>
+      <c r="K16" s="29"/>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A17" s="28"/>
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="28"/>
+      <c r="E17" s="28"/>
+      <c r="F17" s="28"/>
+      <c r="G17" s="28"/>
+      <c r="H17" s="28"/>
+      <c r="I17" s="28"/>
+      <c r="J17" s="28"/>
+      <c r="K17" s="29"/>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A18" s="28"/>
+      <c r="B18" s="28"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="28"/>
+      <c r="E18" s="28"/>
+      <c r="F18" s="28"/>
+      <c r="G18" s="28"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="28"/>
+      <c r="J18" s="28"/>
+      <c r="K18" s="29"/>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A19" s="28"/>
+      <c r="B19" s="28"/>
+      <c r="C19" s="28"/>
+      <c r="D19" s="28"/>
+      <c r="E19" s="28"/>
+      <c r="F19" s="28"/>
+      <c r="G19" s="28"/>
+      <c r="H19" s="28"/>
+      <c r="I19" s="28"/>
+      <c r="J19" s="28"/>
+      <c r="K19" s="29"/>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A20" s="28"/>
+      <c r="B20" s="28"/>
+      <c r="C20" s="28"/>
+      <c r="D20" s="28"/>
+      <c r="E20" s="28"/>
+      <c r="F20" s="28"/>
+      <c r="G20" s="28"/>
+      <c r="H20" s="28"/>
+      <c r="I20" s="28"/>
+      <c r="J20" s="28"/>
+      <c r="K20" s="29"/>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A21" s="43"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A22" s="43"/>
+      <c r="B22" s="43"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
+      <c r="G22" s="43"/>
+      <c r="H22" s="43"/>
+      <c r="I22" s="43"/>
+      <c r="J22" s="43"/>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A23" s="43"/>
+      <c r="B23" s="43"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
+      <c r="G23" s="43"/>
+      <c r="H23" s="43"/>
+      <c r="I23" s="43"/>
+      <c r="J23" s="43"/>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A24" s="43"/>
+      <c r="B24" s="43"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
+      <c r="G24" s="43"/>
+      <c r="H24" s="43"/>
+      <c r="I24" s="43"/>
+      <c r="J24" s="43"/>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="A25" s="43"/>
+      <c r="B25" s="43"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
+      <c r="G25" s="43"/>
+      <c r="H25" s="43"/>
+      <c r="I25" s="43"/>
+      <c r="J25" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A15:A16"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="86" zoomScaleNormal="99" workbookViewId="0">
+    <sheetView topLeftCell="B1" zoomScale="86" zoomScaleNormal="99" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.83984375" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.68359375" style="1" customWidth="1"/>
-    <col min="5" max="5" width="20.578125" style="7" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.7890625" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="13.62890625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5234375" style="7" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="7" customWidth="1"/>
     <col min="7" max="7" width="14" style="1" customWidth="1"/>
-    <col min="8" max="8" width="39.68359375" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.41796875" style="1" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="18.578125" style="7" customWidth="1"/>
-    <col min="11" max="11" width="13.83984375" style="7" customWidth="1"/>
+    <col min="8" max="8" width="39.62890625" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.47265625" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="18.5234375" style="7" customWidth="1"/>
+    <col min="11" max="11" width="13.7890625" style="7" customWidth="1"/>
     <col min="12" max="12" width="10" style="7" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83984375" style="7"/>
+    <col min="13" max="16384" width="8.7890625" style="7"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="6" customFormat="1" x14ac:dyDescent="0.55000000000000004">
@@ -2980,7 +3596,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M12"/>
   <sheetViews>
@@ -2990,17 +3606,17 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" customWidth="1"/>
+    <col min="1" max="1" width="12.47265625" customWidth="1"/>
+    <col min="2" max="2" width="11.5234375" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
-    <col min="6" max="6" width="16.578125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="16.5234375" style="7" customWidth="1"/>
     <col min="7" max="7" width="15.15625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="14.578125" customWidth="1"/>
+    <col min="8" max="8" width="14.5234375" customWidth="1"/>
     <col min="9" max="9" width="38.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="22.83984375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="22.7890625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="13" customWidth="1"/>
-    <col min="12" max="12" width="11.68359375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="9.68359375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.62890625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="9.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.55000000000000004">
@@ -3490,7 +4106,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:L78"/>
   <sheetViews>
@@ -3498,20 +4114,20 @@
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.7890625" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="13.15625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="11.578125" style="1" customWidth="1"/>
-    <col min="3" max="4" width="12.41796875" style="1" customWidth="1"/>
+    <col min="2" max="2" width="11.5234375" style="1" customWidth="1"/>
+    <col min="3" max="4" width="12.47265625" style="1" customWidth="1"/>
     <col min="5" max="5" width="15" style="1" customWidth="1"/>
-    <col min="6" max="6" width="15.41796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.47265625" style="1" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="39.578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="34.578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="12.578125" customWidth="1"/>
-    <col min="11" max="11" width="13.83984375" customWidth="1"/>
+    <col min="8" max="8" width="39.5234375" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="34.5234375" style="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5234375" customWidth="1"/>
+    <col min="11" max="11" width="13.7890625" customWidth="1"/>
     <col min="12" max="12" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="13" max="16384" width="8.83984375" style="1"/>
+    <col min="13" max="16384" width="8.7890625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
@@ -4944,29 +5560,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:K41"/>
+  <dimension ref="A1:L41"/>
   <sheetViews>
-    <sheetView zoomScale="82" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+    <sheetView tabSelected="1" zoomScale="82" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" style="14" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.68359375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.41796875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.47265625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.62890625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.47265625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="13.7890625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.41796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.47265625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="41.26171875" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23.15625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.41796875" customWidth="1"/>
+    <col min="10" max="10" width="12.47265625" customWidth="1"/>
+    <col min="12" max="12" width="19.15625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
@@ -5000,8 +5617,9 @@
       <c r="K1" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+      <c r="L1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A2" s="11">
         <v>1</v>
       </c>
@@ -5036,7 +5654,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -5071,7 +5689,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -5106,7 +5724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -5141,7 +5759,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -5176,7 +5794,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -5211,7 +5829,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -5246,7 +5864,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -5281,7 +5899,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -5316,7 +5934,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -5351,7 +5969,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -5386,7 +6004,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -5421,7 +6039,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -5456,7 +6074,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -5491,7 +6109,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -5650,8 +6268,8 @@
       <c r="F20" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="G20" s="15" t="s">
-        <v>211</v>
+      <c r="G20" s="16" t="s">
+        <v>208</v>
       </c>
       <c r="H20" s="15" t="s">
         <v>212</v>
@@ -5685,8 +6303,8 @@
       <c r="F21" s="15" t="s">
         <v>207</v>
       </c>
-      <c r="G21" s="15" t="s">
-        <v>208</v>
+      <c r="G21" s="16" t="s">
+        <v>211</v>
       </c>
       <c r="H21" s="15" t="s">
         <v>209</v>
@@ -6407,24 +7025,24 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.47265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="15.41796875" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41796875" style="13" customWidth="1"/>
-    <col min="5" max="5" width="15.578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.47265625" style="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.47265625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="15.5234375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="35.41796875" customWidth="1"/>
+    <col min="7" max="7" width="15.5234375" bestFit="1" customWidth="1"/>
+    <col min="8" max="9" width="35.47265625" customWidth="1"/>
     <col min="10" max="10" width="13.15625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -7379,7 +7997,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:L23"/>
   <sheetViews>
@@ -7392,15 +8010,15 @@
     <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.15625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.41796875" customWidth="1"/>
+    <col min="4" max="4" width="15.47265625" customWidth="1"/>
     <col min="5" max="5" width="14.15625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.26171875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="15.26171875" customWidth="1"/>
-    <col min="8" max="8" width="37.41796875" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="37.41796875" customWidth="1"/>
+    <col min="8" max="8" width="37.47265625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="37.47265625" customWidth="1"/>
     <col min="10" max="10" width="14.15625" customWidth="1"/>
-    <col min="11" max="11" width="10.578125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="10.68359375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.5234375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="10.62890625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.55000000000000004">
@@ -8284,7 +8902,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:L17"/>
   <sheetViews>
@@ -8294,16 +8912,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
-    <col min="1" max="1" width="12.41796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.47265625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.15625" customWidth="1"/>
-    <col min="3" max="3" width="15.578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.41796875" customWidth="1"/>
-    <col min="5" max="5" width="13.83984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.5234375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.47265625" customWidth="1"/>
+    <col min="5" max="5" width="13.7890625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15.26171875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="13.68359375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.62890625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="50" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="45.15625" customWidth="1"/>
-    <col min="10" max="10" width="12.83984375" customWidth="1"/>
+    <col min="10" max="10" width="12.7890625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.55000000000000004">

</xml_diff>